<commit_message>
Agregación de plantillas en Input
</commit_message>
<xml_diff>
--- a/Data/Temp/Reporte fidelizaciones Salesforce.xlsx
+++ b/Data/Temp/Reporte fidelizaciones Salesforce.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="31">
   <si>
     <t>Venta: Nombre PDV</t>
   </si>
@@ -93,6 +93,9 @@
     <t>28/03/2022 10:40 AM</t>
   </si>
   <si>
+    <t>Observación</t>
+  </si>
+  <si>
     <t>No. Recibo sin PCC</t>
   </si>
   <si>
@@ -102,19 +105,13 @@
     <t>50000000210344998EDS3234</t>
   </si>
   <si>
-    <t>0000210344998</t>
-  </si>
-  <si>
-    <t>0000210344998EDS3234</t>
-  </si>
-  <si>
-    <t>Observación</t>
-  </si>
-  <si>
     <t>Existe en SalesForce</t>
   </si>
   <si>
     <t>134045454447815243322EDS3226</t>
+  </si>
+  <si>
+    <t>Validación</t>
   </si>
 </sst>
 </file>
@@ -178,11 +175,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -463,224 +462,231 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K6"/>
+  <dimension ref="A1:L6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1:K1048576"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="29" style="3" customWidth="1"/>
-    <col min="3" max="3" width="22" style="3" customWidth="1"/>
-    <col min="4" max="4" width="25" style="3" customWidth="1"/>
-    <col min="5" max="5" width="21" style="3" customWidth="1"/>
-    <col min="6" max="6" width="19" style="3" customWidth="1"/>
-    <col min="7" max="7" width="16" style="3" customWidth="1"/>
-    <col min="8" max="8" width="29" style="3" customWidth="1"/>
-    <col min="9" max="9" width="16" style="3" customWidth="1"/>
-    <col min="10" max="11" width="38" style="3" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="3"/>
+    <col min="3" max="3" width="29" style="5" customWidth="1"/>
+    <col min="4" max="4" width="22" style="3" customWidth="1"/>
+    <col min="5" max="5" width="25" style="3" customWidth="1"/>
+    <col min="6" max="6" width="21" style="3" customWidth="1"/>
+    <col min="7" max="7" width="19" style="3" customWidth="1"/>
+    <col min="8" max="8" width="16" style="3" customWidth="1"/>
+    <col min="9" max="9" width="29" style="3" customWidth="1"/>
+    <col min="10" max="10" width="16" style="3" customWidth="1"/>
+    <col min="11" max="12" width="38" style="3" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>29</v>
-      </c>
     </row>
-    <row r="2" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="4"/>
+      <c r="D2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J2" s="1">
+        <v>10000</v>
+      </c>
+      <c r="K2" s="1"/>
+      <c r="L2" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I2" s="1">
-        <v>10000</v>
-      </c>
-      <c r="J2" s="1"/>
-      <c r="K2" s="2" t="s">
-        <v>30</v>
-      </c>
     </row>
-    <row r="3" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="4"/>
+      <c r="D3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="I3" s="1">
+      <c r="J3" s="1">
         <v>10000</v>
       </c>
-      <c r="J3" s="1"/>
-      <c r="K3" s="2" t="s">
-        <v>30</v>
+      <c r="K3" s="1"/>
+      <c r="L3" s="2" t="s">
+        <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="C4" s="4"/>
+      <c r="D4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J4" s="1">
+        <v>10000</v>
+      </c>
+      <c r="K4" s="1"/>
+      <c r="L4" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I4" s="1">
-        <v>10000</v>
-      </c>
-      <c r="J4" s="1"/>
-      <c r="K4" s="2" t="s">
-        <v>30</v>
-      </c>
     </row>
-    <row r="5" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" s="4"/>
+      <c r="D5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="G5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="H5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="I5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="I5" s="1">
+      <c r="J5" s="1">
         <v>10000</v>
       </c>
-      <c r="J5" s="1"/>
-      <c r="K5" s="2" t="s">
-        <v>30</v>
+      <c r="K5" s="1"/>
+      <c r="L5" s="2" t="s">
+        <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" s="4"/>
+      <c r="D6" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="E6" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="F6" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="G6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="H6" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="I6" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="I6" s="1">
+      <c r="J6" s="1">
         <v>5000</v>
       </c>
-      <c r="J6" s="1"/>
-      <c r="K6" s="2" t="s">
-        <v>30</v>
+      <c r="K6" s="1"/>
+      <c r="L6" s="2" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
arreglo de funciones para lectura de archivo excel
</commit_message>
<xml_diff>
--- a/Data/Temp/Reporte fidelizaciones Salesforce.xlsx
+++ b/Data/Temp/Reporte fidelizaciones Salesforce.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Validación ventas redencion R" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="33">
   <si>
     <t>Venta: Nombre PDV</t>
   </si>
@@ -116,6 +116,9 @@
   </si>
   <si>
     <t>Existe en Satelite</t>
+  </si>
+  <si>
+    <t>No Existe en Satelite</t>
   </si>
 </sst>
 </file>
@@ -470,7 +473,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -481,10 +484,10 @@
   <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="2" width="29" style="3" customWidth="1"/>
     <col min="3" max="3" width="29" style="5" customWidth="1"/>
@@ -496,10 +499,10 @@
     <col min="9" max="9" width="29" style="3" customWidth="1"/>
     <col min="10" max="10" width="16" style="3" customWidth="1"/>
     <col min="11" max="12" width="38" style="3" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="3"/>
+    <col min="13" max="16384" width="9.1796875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>25</v>
       </c>
@@ -537,7 +540,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
       <c r="B2" s="1">
         <v>1</v>
@@ -555,7 +558,7 @@
       <c r="K2" s="1"/>
       <c r="L2" s="2"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
@@ -563,7 +566,7 @@
         <v>27</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>9</v>
@@ -591,7 +594,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -599,7 +602,7 @@
         <v>27</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>9</v>
@@ -627,7 +630,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -635,7 +638,7 @@
         <v>27</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>9</v>
@@ -663,7 +666,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -671,7 +674,7 @@
         <v>27</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>9</v>
@@ -699,7 +702,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>18</v>
       </c>
@@ -707,7 +710,7 @@
         <v>29</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>19</v>

</xml_diff>

<commit_message>
Cambios archivo extracion novedades
</commit_message>
<xml_diff>
--- a/Data/Temp/Reporte fidelizaciones Salesforce.xlsx
+++ b/Data/Temp/Reporte fidelizaciones Salesforce.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="30">
   <si>
     <t>Venta: Nombre PDV</t>
   </si>
@@ -110,15 +110,6 @@
   </si>
   <si>
     <t>134045454447815243322EDS3226</t>
-  </si>
-  <si>
-    <t>Validación</t>
-  </si>
-  <si>
-    <t>Existe en Satelite</t>
-  </si>
-  <si>
-    <t>No Existe en Satelite</t>
   </si>
 </sst>
 </file>
@@ -182,13 +173,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -481,7 +470,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L7"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C1" sqref="C1:C1048576"/>
@@ -490,64 +479,58 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="2" width="29" style="3" customWidth="1"/>
-    <col min="3" max="3" width="29" style="5" customWidth="1"/>
-    <col min="4" max="4" width="22" style="3" customWidth="1"/>
-    <col min="5" max="5" width="25" style="3" customWidth="1"/>
-    <col min="6" max="6" width="21" style="3" customWidth="1"/>
-    <col min="7" max="7" width="19" style="3" customWidth="1"/>
-    <col min="8" max="8" width="16" style="3" customWidth="1"/>
-    <col min="9" max="9" width="29" style="3" customWidth="1"/>
-    <col min="10" max="10" width="16" style="3" customWidth="1"/>
-    <col min="11" max="12" width="38" style="3" customWidth="1"/>
-    <col min="13" max="16384" width="9.1796875" style="3"/>
+    <col min="3" max="3" width="22" style="3" customWidth="1"/>
+    <col min="4" max="4" width="25" style="3" customWidth="1"/>
+    <col min="5" max="5" width="21" style="3" customWidth="1"/>
+    <col min="6" max="6" width="19" style="3" customWidth="1"/>
+    <col min="7" max="7" width="16" style="3" customWidth="1"/>
+    <col min="8" max="8" width="29" style="3" customWidth="1"/>
+    <col min="9" max="9" width="16" style="3" customWidth="1"/>
+    <col min="10" max="11" width="38" style="3" customWidth="1"/>
+    <col min="12" max="16384" width="9.1796875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>30</v>
+      <c r="C1" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="K1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
       <c r="B2" s="1">
         <v>1</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>31</v>
-      </c>
+      <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
@@ -555,186 +538,170 @@
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="2"/>
+      <c r="K2" s="2"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>32</v>
+      <c r="C3" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="J3" s="1">
+      <c r="I3" s="1">
         <v>10000</v>
       </c>
-      <c r="K3" s="1"/>
-      <c r="L3" s="2" t="s">
+      <c r="J3" s="1"/>
+      <c r="K3" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>32</v>
+      <c r="C4" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="I4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="J4" s="1">
+      <c r="I4" s="1">
         <v>10000</v>
       </c>
-      <c r="K4" s="1"/>
-      <c r="L4" s="2" t="s">
+      <c r="J4" s="1"/>
+      <c r="K4" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C5" s="4" t="s">
-        <v>32</v>
+      <c r="C5" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="J5" s="1">
+      <c r="I5" s="1">
         <v>10000</v>
       </c>
-      <c r="K5" s="1"/>
-      <c r="L5" s="2" t="s">
+      <c r="J5" s="1"/>
+      <c r="K5" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="4" t="s">
-        <v>32</v>
+      <c r="C6" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="J6" s="1">
+      <c r="I6" s="1">
         <v>10000</v>
       </c>
-      <c r="K6" s="1"/>
-      <c r="L6" s="2" t="s">
+      <c r="J6" s="1"/>
+      <c r="K6" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C7" s="4" t="s">
-        <v>32</v>
+      <c r="C7" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="I7" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="J7" s="1">
+      <c r="I7" s="1">
         <v>5000</v>
       </c>
-      <c r="K7" s="1"/>
-      <c r="L7" s="2" t="s">
+      <c r="J7" s="1"/>
+      <c r="K7" s="2" t="s">
         <v>28</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Correcciones 3, 6 finalización  8, 9
</commit_message>
<xml_diff>
--- a/Data/Temp/Reporte fidelizaciones Salesforce.xlsx
+++ b/Data/Temp/Reporte fidelizaciones Salesforce.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="41">
   <si>
     <t>Venta: Nombre PDV</t>
   </si>
@@ -140,6 +140,9 @@
   </si>
   <si>
     <t>EDS2231</t>
+  </si>
+  <si>
+    <t>5215EDS3225</t>
   </si>
 </sst>
 </file>
@@ -524,7 +527,7 @@
   <dimension ref="A1:L37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13:E22"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1233,7 +1236,7 @@
         <v>5.0000000210344896E+16</v>
       </c>
       <c r="B20" t="s">
-        <v>19</v>
+        <v>40</v>
       </c>
       <c r="C20" t="s">
         <v>29</v>

</xml_diff>